<commit_message>
A basic finished codes for Exp2-1, Exp2-2, Exp2-3-ParzenWindow and Exp2-3-KNN!
</commit_message>
<xml_diff>
--- a/Exp2/data/exp2-3.xlsx
+++ b/Exp2/data/exp2-3.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ExpMachineLearn\ExpML\Exp2\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815628B7-EF58-4211-8440-08F479581569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +24,40 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>x1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -53,7 +85,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +362,451 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B2">
+        <v>1.31</v>
+      </c>
+      <c r="C2">
+        <v>-6.2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B3">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C3">
+        <v>-0.78</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1.54</v>
+      </c>
+      <c r="B4">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C4">
+        <v>-1.63</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-0.44</v>
+      </c>
+      <c r="B5">
+        <v>1.18</v>
+      </c>
+      <c r="C5">
+        <v>-4.32</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-0.81</v>
+      </c>
+      <c r="B6">
+        <v>0.21</v>
+      </c>
+      <c r="C6">
+        <v>5.73</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.52</v>
+      </c>
+      <c r="B7">
+        <v>3.16</v>
+      </c>
+      <c r="C7">
+        <v>2.77</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B8">
+        <v>2.42</v>
+      </c>
+      <c r="C8">
+        <v>-0.19</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.91</v>
+      </c>
+      <c r="B9">
+        <v>1.94</v>
+      </c>
+      <c r="C9">
+        <v>6.21</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.65</v>
+      </c>
+      <c r="B10">
+        <v>1.93</v>
+      </c>
+      <c r="C10">
+        <v>4.38</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-0.26</v>
+      </c>
+      <c r="B11">
+        <v>0.82</v>
+      </c>
+      <c r="C11">
+        <v>-0.96</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="B12">
+        <v>1.03</v>
+      </c>
+      <c r="C12">
+        <v>-0.21</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1.27</v>
+      </c>
+      <c r="B13">
+        <v>1.28</v>
+      </c>
+      <c r="C13">
+        <v>0.08</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.13</v>
+      </c>
+      <c r="B14">
+        <v>3.12</v>
+      </c>
+      <c r="C14">
+        <v>0.16</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-0.21</v>
+      </c>
+      <c r="B15">
+        <v>1.23</v>
+      </c>
+      <c r="C15">
+        <v>-0.11</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-2.1800000000000002</v>
+      </c>
+      <c r="B16">
+        <v>1.39</v>
+      </c>
+      <c r="C16">
+        <v>-0.19</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.34</v>
+      </c>
+      <c r="B17">
+        <v>1.96</v>
+      </c>
+      <c r="C17">
+        <v>-0.16</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-1.38</v>
+      </c>
+      <c r="B18">
+        <v>0.94</v>
+      </c>
+      <c r="C18">
+        <v>0.45</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>-0.12</v>
+      </c>
+      <c r="B19">
+        <v>0.82</v>
+      </c>
+      <c r="C19">
+        <v>0.17</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-1.44</v>
+      </c>
+      <c r="B20">
+        <v>2.31</v>
+      </c>
+      <c r="C20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.26</v>
+      </c>
+      <c r="B21">
+        <v>1.94</v>
+      </c>
+      <c r="C21">
+        <v>0.08</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1.36</v>
+      </c>
+      <c r="B22">
+        <v>2.17</v>
+      </c>
+      <c r="C22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1.41</v>
+      </c>
+      <c r="B23">
+        <v>1.45</v>
+      </c>
+      <c r="C23">
+        <v>-0.38</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1.22</v>
+      </c>
+      <c r="B24">
+        <v>0.99</v>
+      </c>
+      <c r="C24">
+        <v>0.69</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2.46</v>
+      </c>
+      <c r="B25">
+        <v>2.19</v>
+      </c>
+      <c r="C25">
+        <v>1.31</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.68</v>
+      </c>
+      <c r="B26">
+        <v>0.79</v>
+      </c>
+      <c r="C26">
+        <v>0.87</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="B27">
+        <v>3.22</v>
+      </c>
+      <c r="C27">
+        <v>1.35</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.6</v>
+      </c>
+      <c r="B28">
+        <v>2.44</v>
+      </c>
+      <c r="C28">
+        <v>0.92</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.64</v>
+      </c>
+      <c r="B29">
+        <v>0.13</v>
+      </c>
+      <c r="C29">
+        <v>0.97</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.85</v>
+      </c>
+      <c r="B30">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C30">
+        <v>0.99</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.66</v>
+      </c>
+      <c r="B31">
+        <v>0.51</v>
+      </c>
+      <c r="C31">
+        <v>0.88</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>